<commit_message>
T1 initial + ESP livingroom
</commit_message>
<xml_diff>
--- a/other/ItemList.xlsx
+++ b/other/ItemList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="0" windowWidth="21570" windowHeight="6465" xr2:uid="{2BD6B4C2-05D5-4663-BC50-E29FAF3AB66F}"/>
+    <workbookView xWindow="4230" yWindow="0" windowWidth="21570" windowHeight="6465" xr2:uid="{2BD6B4C2-05D5-4663-BC50-E29FAF3AB66F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="101">
   <si>
     <t>Przedpokój</t>
   </si>
@@ -303,6 +303,30 @@
   </si>
   <si>
     <t>https://www.gearbest.com/ceiling-lights/pp_596249.html?utm_source=tt_de&amp;aid=171752</t>
+  </si>
+  <si>
+    <t>Samsung BRB260087WW</t>
+  </si>
+  <si>
+    <t>Samsung DW50K4050BB</t>
+  </si>
+  <si>
+    <t>Różnica w estymatach</t>
+  </si>
+  <si>
+    <t>Samsung NQ50H5537KB</t>
+  </si>
+  <si>
+    <t>Samsung NZ64K7757BK</t>
+  </si>
+  <si>
+    <t>Samsung NK24M5070BG</t>
+  </si>
+  <si>
+    <t>Piekarnik z mikrofala</t>
+  </si>
+  <si>
+    <t>https://www.gearbest.com/flush-ceiling-lights/pp_1119130.html</t>
   </si>
 </sst>
 </file>
@@ -712,10 +736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648B1029-8A81-4C9E-B117-6F0610D1C64B}">
-  <dimension ref="D2:P79"/>
+  <dimension ref="D2:Q79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="W35" sqref="W35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,15 +756,16 @@
     <col min="14" max="14" width="12.140625" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
     <col min="16" max="16" width="14.28515625" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:17" x14ac:dyDescent="0.25">
       <c r="J2">
         <f>60/2.5</f>
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:17" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
         <v>65</v>
       </c>
@@ -755,7 +780,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>68</v>
       </c>
@@ -766,7 +791,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:17" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
         <v>26</v>
       </c>
@@ -777,7 +802,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="4:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -797,8 +822,11 @@
       <c r="P6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="7" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="Q6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
@@ -822,8 +850,9 @@
       <c r="N7" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="8" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>79</v>
       </c>
@@ -856,8 +885,9 @@
         <f>($H8/$H$4)*L8</f>
         <v>432</v>
       </c>
-    </row>
-    <row r="9" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>79</v>
       </c>
@@ -887,8 +917,9 @@
         <f>($H9/$H$3)*L9</f>
         <v>37.200000000000003</v>
       </c>
-    </row>
-    <row r="10" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>80</v>
       </c>
@@ -921,8 +952,9 @@
         <f>H10*L10</f>
         <v>1300</v>
       </c>
-    </row>
-    <row r="11" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>80</v>
       </c>
@@ -955,8 +987,9 @@
         <f>$H11*L11</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>80</v>
       </c>
@@ -986,8 +1019,9 @@
         <f>$H12*L12</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>0</v>
       </c>
@@ -1014,8 +1048,9 @@
         <f>H13*L13</f>
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F14" s="4" t="s">
         <v>0</v>
       </c>
@@ -1033,8 +1068,9 @@
       <c r="L14" s="4"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
-    </row>
-    <row r="15" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>79</v>
       </c>
@@ -1070,8 +1106,12 @@
       <c r="P15">
         <v>260</v>
       </c>
-    </row>
-    <row r="16" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="Q15" s="2">
+        <f t="shared" ref="Q15:Q64" si="0">P15-N15</f>
+        <v>-340</v>
+      </c>
+    </row>
+    <row r="16" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>0</v>
       </c>
@@ -1098,8 +1138,9 @@
         <f>H16*L16</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>79</v>
       </c>
@@ -1132,8 +1173,9 @@
         <f>($H17/$H$4)*L17</f>
         <v>496.79999999999995</v>
       </c>
-    </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>79</v>
       </c>
@@ -1166,8 +1208,9 @@
         <f>($H18/$H$4)*L18</f>
         <v>2100</v>
       </c>
-    </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>79</v>
       </c>
@@ -1197,8 +1240,18 @@
         <f>H19*L19</f>
         <v>680</v>
       </c>
-    </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>92</v>
+      </c>
+      <c r="P19">
+        <v>260</v>
+      </c>
+      <c r="Q19" s="2">
+        <f t="shared" ref="Q19" si="1">P19-N19</f>
+        <v>-420</v>
+      </c>
+    </row>
+    <row r="20" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>79</v>
       </c>
@@ -1228,11 +1281,12 @@
         <v>1000</v>
       </c>
       <c r="N20" s="2">
-        <f t="shared" ref="N20:N26" si="0">$H20*L20</f>
+        <f t="shared" ref="N20:N26" si="2">$H20*L20</f>
         <v>1500</v>
       </c>
-    </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>79</v>
       </c>
@@ -1258,15 +1312,16 @@
         <v>1000</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" ref="M21:M26" si="1">$H21*K21</f>
+        <f t="shared" ref="M21:M26" si="3">$H21*K21</f>
         <v>1000</v>
       </c>
       <c r="N21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1000</v>
       </c>
-    </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>79</v>
       </c>
@@ -1289,15 +1344,16 @@
         <v>1600</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1000</v>
       </c>
       <c r="N22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1600</v>
       </c>
-    </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>79</v>
       </c>
@@ -1320,15 +1376,16 @@
         <v>100</v>
       </c>
       <c r="M23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="N23" s="2">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>79</v>
       </c>
@@ -1351,15 +1408,16 @@
         <v>100</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="N24" s="2">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>79</v>
       </c>
@@ -1382,15 +1440,16 @@
         <v>100</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="N25" s="2">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>80</v>
       </c>
@@ -1416,15 +1475,16 @@
         <v>1500</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1300</v>
       </c>
       <c r="N26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1500</v>
       </c>
-    </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q26" s="2"/>
+    </row>
+    <row r="27" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>79</v>
       </c>
@@ -1447,15 +1507,16 @@
         <v>900</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" ref="M27:M29" si="2">$H27*K27</f>
+        <f t="shared" ref="M27:M29" si="4">$H27*K27</f>
         <v>700</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" ref="N27:N29" si="3">$H27*L27</f>
+        <f t="shared" ref="N27:N29" si="5">$H27*L27</f>
         <v>900</v>
       </c>
-    </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>80</v>
       </c>
@@ -1484,15 +1545,16 @@
         <v>100</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="N28" s="2">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="Q28" s="2"/>
+    </row>
+    <row r="29" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>81</v>
       </c>
@@ -1518,15 +1580,16 @@
         <v>3500</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2500</v>
       </c>
       <c r="N29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3500</v>
       </c>
-    </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F30" s="4" t="s">
         <v>1</v>
       </c>
@@ -1544,8 +1607,9 @@
       <c r="L30" s="4"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
-    </row>
-    <row r="31" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>79</v>
       </c>
@@ -1578,8 +1642,9 @@
         <f>($H31/$H$5)*L31</f>
         <v>1090</v>
       </c>
-    </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q31" s="2"/>
+    </row>
+    <row r="32" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>79</v>
       </c>
@@ -1602,15 +1667,16 @@
         <v>24</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" ref="M32:M54" si="4">($H32/$H$3)*K32</f>
+        <f t="shared" ref="M32:M54" si="6">($H32/$H$3)*K32</f>
         <v>51.36</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" ref="N32:N54" si="5">($H32/$H$3)*L32</f>
+        <f t="shared" ref="N32:N54" si="7">($H32/$H$3)*L32</f>
         <v>77.039999999999992</v>
       </c>
-    </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q32" s="2"/>
+    </row>
+    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E33" s="9"/>
       <c r="F33" t="s">
         <v>2</v>
@@ -1631,15 +1697,16 @@
         <v>4500</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" ref="M33" si="6">$H33*K33</f>
+        <f t="shared" ref="M33" si="8">$H33*K33</f>
         <v>3000</v>
       </c>
       <c r="N33" s="2">
-        <f t="shared" ref="N33" si="7">$H33*L33</f>
+        <f t="shared" ref="N33" si="9">$H33*L33</f>
         <v>4500</v>
       </c>
-    </row>
-    <row r="34" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q33" s="2"/>
+    </row>
+    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
         <v>2</v>
       </c>
@@ -1647,7 +1714,7 @@
         <v>28</v>
       </c>
       <c r="H34">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="I34" t="s">
         <v>64</v>
@@ -1659,15 +1726,25 @@
         <v>100</v>
       </c>
       <c r="M34">
-        <f t="shared" ref="M34:M38" si="8">$H34*K34</f>
-        <v>3000</v>
+        <f t="shared" ref="M34:M38" si="10">$H34*K34</f>
+        <v>900</v>
       </c>
       <c r="N34">
-        <f t="shared" ref="N34:N38" si="9">$H34*L34</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" ref="N34:N38" si="11">$H34*L34</f>
+        <v>900</v>
+      </c>
+      <c r="O34" t="s">
+        <v>92</v>
+      </c>
+      <c r="P34">
+        <v>260</v>
+      </c>
+      <c r="Q34" s="2">
+        <f>P34-N34</f>
+        <v>-640</v>
+      </c>
+    </row>
+    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
         <v>2</v>
       </c>
@@ -1687,15 +1764,16 @@
         <v>100</v>
       </c>
       <c r="M35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>200</v>
       </c>
       <c r="N35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="36" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q35" s="2"/>
+    </row>
+    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
         <v>2</v>
       </c>
@@ -1715,15 +1793,16 @@
         <v>65</v>
       </c>
       <c r="M36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>65</v>
       </c>
       <c r="N36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="37" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q36" s="2"/>
+    </row>
+    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>80</v>
       </c>
@@ -1752,15 +1831,16 @@
         <v>600</v>
       </c>
       <c r="M37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>150</v>
       </c>
       <c r="N37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>600</v>
       </c>
-    </row>
-    <row r="38" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q37" s="2"/>
+    </row>
+    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E38" s="10"/>
       <c r="F38" t="s">
         <v>2</v>
@@ -1781,15 +1861,16 @@
         <v>300</v>
       </c>
       <c r="M38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>150</v>
       </c>
       <c r="N38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>300</v>
       </c>
-    </row>
-    <row r="39" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q38" s="2"/>
+    </row>
+    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F39" s="4" t="s">
         <v>2</v>
       </c>
@@ -1807,8 +1888,9 @@
       <c r="L39" s="4"/>
       <c r="M39" s="5"/>
       <c r="N39" s="5"/>
-    </row>
-    <row r="40" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q39" s="2"/>
+    </row>
+    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>79</v>
       </c>
@@ -1841,8 +1923,9 @@
         <f>($H40/$H$5)*L40</f>
         <v>1900</v>
       </c>
-    </row>
-    <row r="41" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q40" s="2"/>
+    </row>
+    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>79</v>
       </c>
@@ -1868,15 +1951,16 @@
         <v>24</v>
       </c>
       <c r="M41" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>48.96</v>
       </c>
       <c r="N41" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>73.44</v>
       </c>
-    </row>
-    <row r="42" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q41" s="2"/>
+    </row>
+    <row r="42" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>79</v>
       </c>
@@ -1887,7 +1971,7 @@
         <v>28</v>
       </c>
       <c r="H42">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="I42" t="s">
         <v>64</v>
@@ -1899,15 +1983,25 @@
         <v>100</v>
       </c>
       <c r="M42">
-        <f t="shared" ref="M42" si="10">$H42*K42</f>
-        <v>900</v>
+        <f t="shared" ref="M42" si="12">$H42*K42</f>
+        <v>3000</v>
       </c>
       <c r="N42">
-        <f t="shared" ref="N42" si="11">$H42*L42</f>
-        <v>900</v>
-      </c>
-    </row>
-    <row r="43" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" ref="N42" si="13">$H42*L42</f>
+        <v>3000</v>
+      </c>
+      <c r="O42" t="s">
+        <v>100</v>
+      </c>
+      <c r="P42">
+        <v>600</v>
+      </c>
+      <c r="Q42" s="2">
+        <f>P42-N42</f>
+        <v>-2400</v>
+      </c>
+    </row>
+    <row r="43" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>79</v>
       </c>
@@ -1930,15 +2024,16 @@
         <v>65</v>
       </c>
       <c r="M43">
-        <f t="shared" ref="M43:M47" si="12">$H43*K43</f>
+        <f t="shared" ref="M43:M47" si="14">$H43*K43</f>
         <v>65</v>
       </c>
       <c r="N43">
-        <f t="shared" ref="N43:N47" si="13">$H43*L43</f>
+        <f t="shared" ref="N43:N47" si="15">$H43*L43</f>
         <v>65</v>
       </c>
-    </row>
-    <row r="44" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q43" s="2"/>
+    </row>
+    <row r="44" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>80</v>
       </c>
@@ -1961,15 +2056,16 @@
         <v>1200</v>
       </c>
       <c r="M44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>500</v>
       </c>
       <c r="N44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1200</v>
       </c>
-    </row>
-    <row r="45" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q44" s="2"/>
+    </row>
+    <row r="45" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>80</v>
       </c>
@@ -1992,15 +2088,16 @@
         <v>4000</v>
       </c>
       <c r="M45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1000</v>
       </c>
       <c r="N45">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4000</v>
       </c>
-    </row>
-    <row r="46" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q45" s="2"/>
+    </row>
+    <row r="46" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
         <v>80</v>
       </c>
@@ -2026,15 +2123,16 @@
         <v>400</v>
       </c>
       <c r="M46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>150</v>
       </c>
       <c r="N46">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>400</v>
       </c>
-    </row>
-    <row r="47" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q46" s="2"/>
+    </row>
+    <row r="47" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E47" s="10"/>
       <c r="F47" t="s">
         <v>4</v>
@@ -2055,15 +2153,16 @@
         <v>300</v>
       </c>
       <c r="M47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>600</v>
       </c>
       <c r="N47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>1200</v>
       </c>
-    </row>
-    <row r="48" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q47" s="2"/>
+    </row>
+    <row r="48" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F48" s="4" t="s">
         <v>4</v>
       </c>
@@ -2081,8 +2180,9 @@
       <c r="L48" s="4"/>
       <c r="M48" s="5"/>
       <c r="N48" s="5"/>
-    </row>
-    <row r="49" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q48" s="2"/>
+    </row>
+    <row r="49" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
         <v>79</v>
       </c>
@@ -2115,8 +2215,9 @@
         <f>($H49/$H$4)*L49</f>
         <v>1998</v>
       </c>
-    </row>
-    <row r="50" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q49" s="2"/>
+    </row>
+    <row r="50" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
         <v>79</v>
       </c>
@@ -2142,15 +2243,16 @@
         <v>24</v>
       </c>
       <c r="M50" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>89.6</v>
       </c>
       <c r="N50" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>134.39999999999998</v>
       </c>
-    </row>
-    <row r="51" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q50" s="2"/>
+    </row>
+    <row r="51" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
         <v>79</v>
       </c>
@@ -2183,8 +2285,9 @@
         <f>$H51*L51</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="52" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q51" s="2"/>
+    </row>
+    <row r="52" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
         <v>79</v>
       </c>
@@ -2214,11 +2317,12 @@
         <v>100</v>
       </c>
       <c r="N52" s="2">
-        <f t="shared" ref="N52" si="14">$H52*L52</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="4:14" x14ac:dyDescent="0.25">
+        <f t="shared" ref="N52" si="16">$H52*L52</f>
+        <v>100</v>
+      </c>
+      <c r="Q52" s="2"/>
+    </row>
+    <row r="53" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
         <v>79</v>
       </c>
@@ -2251,8 +2355,9 @@
         <f>($H53/$H$4)*L53</f>
         <v>572.4</v>
       </c>
-    </row>
-    <row r="54" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q53" s="2"/>
+    </row>
+    <row r="54" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
         <v>79</v>
       </c>
@@ -2275,15 +2380,16 @@
         <v>24</v>
       </c>
       <c r="M54" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>26.72</v>
       </c>
       <c r="N54" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>40.08</v>
       </c>
-    </row>
-    <row r="55" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q54" s="2"/>
+    </row>
+    <row r="55" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>79</v>
       </c>
@@ -2312,15 +2418,16 @@
         <v>10000</v>
       </c>
       <c r="M55" s="7">
-        <f t="shared" ref="M55" si="15">$H55*K55</f>
+        <f t="shared" ref="M55" si="17">$H55*K55</f>
         <v>9400</v>
       </c>
       <c r="N55" s="7">
-        <f t="shared" ref="N55" si="16">$H55*L55</f>
+        <f t="shared" ref="N55" si="18">$H55*L55</f>
         <v>10000</v>
       </c>
-    </row>
-    <row r="56" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q55" s="2"/>
+    </row>
+    <row r="56" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
         <v>81</v>
       </c>
@@ -2346,15 +2453,25 @@
         <v>3500</v>
       </c>
       <c r="M56" s="2">
-        <f t="shared" ref="M56:M59" si="17">$H56*K56</f>
+        <f t="shared" ref="M56:M59" si="19">$H56*K56</f>
         <v>2000</v>
       </c>
       <c r="N56" s="2">
-        <f t="shared" ref="N56:N59" si="18">$H56*L56</f>
+        <f t="shared" ref="N56:N59" si="20">$H56*L56</f>
         <v>3500</v>
       </c>
-    </row>
-    <row r="57" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="O56" t="s">
+        <v>93</v>
+      </c>
+      <c r="P56">
+        <v>2900</v>
+      </c>
+      <c r="Q56" s="2">
+        <f t="shared" si="0"/>
+        <v>-600</v>
+      </c>
+    </row>
+    <row r="57" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
         <v>81</v>
       </c>
@@ -2380,15 +2497,25 @@
         <v>2500</v>
       </c>
       <c r="M57" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1500</v>
       </c>
       <c r="N57" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>2500</v>
       </c>
-    </row>
-    <row r="58" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="O57" t="s">
+        <v>96</v>
+      </c>
+      <c r="P57">
+        <v>1900</v>
+      </c>
+      <c r="Q57" s="2">
+        <f t="shared" si="0"/>
+        <v>-600</v>
+      </c>
+    </row>
+    <row r="58" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
         <v>81</v>
       </c>
@@ -2414,15 +2541,25 @@
         <v>1700</v>
       </c>
       <c r="M58" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>900</v>
       </c>
       <c r="N58" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>1700</v>
       </c>
-    </row>
-    <row r="59" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="O58" t="s">
+        <v>99</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="2">
+        <f t="shared" si="0"/>
+        <v>-1700</v>
+      </c>
+    </row>
+    <row r="59" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
         <v>81</v>
       </c>
@@ -2448,15 +2585,25 @@
         <v>2300</v>
       </c>
       <c r="M59" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1500</v>
       </c>
       <c r="N59" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>2300</v>
       </c>
-    </row>
-    <row r="60" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="O59" t="s">
+        <v>94</v>
+      </c>
+      <c r="P59">
+        <v>1300</v>
+      </c>
+      <c r="Q59" s="2">
+        <f t="shared" si="0"/>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="60" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
         <v>81</v>
       </c>
@@ -2482,15 +2629,25 @@
         <v>1600</v>
       </c>
       <c r="M60" s="2">
-        <f t="shared" ref="M60:N64" si="19">$H60*K60</f>
+        <f t="shared" ref="M60:N64" si="21">$H60*K60</f>
         <v>500</v>
       </c>
       <c r="N60" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1600</v>
       </c>
-    </row>
-    <row r="61" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="O60" t="s">
+        <v>98</v>
+      </c>
+      <c r="P60">
+        <v>1400</v>
+      </c>
+      <c r="Q60" s="2">
+        <f t="shared" si="0"/>
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="61" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
         <v>81</v>
       </c>
@@ -2513,15 +2670,16 @@
         <v>150</v>
       </c>
       <c r="M61" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>100</v>
       </c>
       <c r="N61" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>150</v>
       </c>
-    </row>
-    <row r="62" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="Q61" s="2"/>
+    </row>
+    <row r="62" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
         <v>81</v>
       </c>
@@ -2544,15 +2702,25 @@
         <v>1900</v>
       </c>
       <c r="M62" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1500</v>
       </c>
       <c r="N62" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>1900</v>
       </c>
-    </row>
-    <row r="63" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="O62" t="s">
+        <v>97</v>
+      </c>
+      <c r="P62">
+        <v>2000</v>
+      </c>
+      <c r="Q62" s="2">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
         <v>79</v>
       </c>
@@ -2575,15 +2743,25 @@
         <v>500</v>
       </c>
       <c r="M63" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>500</v>
       </c>
       <c r="N63" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>500</v>
       </c>
-    </row>
-    <row r="64" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="O63" t="s">
+        <v>92</v>
+      </c>
+      <c r="P63">
+        <v>260</v>
+      </c>
+      <c r="Q63" s="2">
+        <f t="shared" ref="Q63" si="22">P63-N63</f>
+        <v>-240</v>
+      </c>
+    </row>
+    <row r="64" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
         <v>3</v>
       </c>
@@ -2606,15 +2784,16 @@
         <v>100</v>
       </c>
       <c r="M64">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>300</v>
       </c>
       <c r="N64">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>300</v>
       </c>
-    </row>
-    <row r="65" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="Q64" s="2"/>
+    </row>
+    <row r="65" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F65" s="13" t="s">
         <v>67</v>
       </c>
@@ -2632,8 +2811,16 @@
         <f>SUM(N8:N64)</f>
         <v>64226.36</v>
       </c>
-    </row>
-    <row r="66" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="P65" s="2">
+        <f>SUM(P8:P64)</f>
+        <v>11140</v>
+      </c>
+      <c r="Q65" s="2">
+        <f>SUM(Q8:Q64)</f>
+        <v>-8040</v>
+      </c>
+    </row>
+    <row r="66" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F66" s="12" t="s">
         <v>70</v>
       </c>
@@ -2652,7 +2839,7 @@
         <v>61993.96</v>
       </c>
     </row>
-    <row r="67" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F67" s="12" t="s">
         <v>71</v>
       </c>
@@ -2671,7 +2858,7 @@
         <v>2232.4</v>
       </c>
     </row>
-    <row r="73" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="6:17" x14ac:dyDescent="0.25">
       <c r="M73" t="s">
         <v>3</v>
       </c>
@@ -2680,7 +2867,7 @@
         <v>25062.48</v>
       </c>
     </row>
-    <row r="74" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="6:17" x14ac:dyDescent="0.25">
       <c r="M74" t="s">
         <v>87</v>
       </c>
@@ -2689,16 +2876,16 @@
         <v>13676.8</v>
       </c>
     </row>
-    <row r="75" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="6:17" x14ac:dyDescent="0.25">
       <c r="M75" t="s">
         <v>88</v>
       </c>
       <c r="N75" s="2">
         <f>SUM(N40:N48)</f>
-        <v>9738.44</v>
-      </c>
-    </row>
-    <row r="76" spans="6:14" x14ac:dyDescent="0.25">
+        <v>11838.44</v>
+      </c>
+    </row>
+    <row r="76" spans="6:17" x14ac:dyDescent="0.25">
       <c r="M76" t="s">
         <v>89</v>
       </c>
@@ -2707,16 +2894,16 @@
         <v>3584.2</v>
       </c>
     </row>
-    <row r="77" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="6:17" x14ac:dyDescent="0.25">
       <c r="M77" t="s">
         <v>2</v>
       </c>
       <c r="N77" s="2">
         <f>SUM(N31:N39)</f>
-        <v>9832.0400000000009</v>
-      </c>
-    </row>
-    <row r="78" spans="6:14" x14ac:dyDescent="0.25">
+        <v>7732.04</v>
+      </c>
+    </row>
+    <row r="78" spans="6:17" x14ac:dyDescent="0.25">
       <c r="M78" t="s">
         <v>5</v>
       </c>
@@ -2725,7 +2912,7 @@
         <v>2232.4</v>
       </c>
     </row>
-    <row r="79" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="6:17" x14ac:dyDescent="0.25">
       <c r="M79" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
calendar day in week update
</commit_message>
<xml_diff>
--- a/other/ItemList.xlsx
+++ b/other/ItemList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FW_Allowed\GithubProjects\OpenHabHomeAutomation\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DE4107-91B2-4241-83A2-4CCEB110C7A3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B504B69E-0F20-44B5-93DB-AF8D6E02DAB6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="0" windowWidth="21570" windowHeight="6465" activeTab="3" xr2:uid="{2BD6B4C2-05D5-4663-BC50-E29FAF3AB66F}"/>
+    <workbookView xWindow="12690" yWindow="0" windowWidth="21570" windowHeight="6465" activeTab="3" xr2:uid="{2BD6B4C2-05D5-4663-BC50-E29FAF3AB66F}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemList" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="144">
   <si>
     <t>Przedpokój</t>
   </si>
@@ -445,6 +445,21 @@
   </si>
   <si>
     <t>Najważniejsze+kuchnia</t>
+  </si>
+  <si>
+    <t>35k,6k</t>
+  </si>
+  <si>
+    <t>22k</t>
+  </si>
+  <si>
+    <t>22k - 25k</t>
+  </si>
+  <si>
+    <t>+ekipa remontowa</t>
+  </si>
+  <si>
+    <t>w tym 17k/lub23k na remont</t>
   </si>
 </sst>
 </file>
@@ -519,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -534,13 +549,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648B1029-8A81-4C9E-B117-6F0610D1C64B}">
-  <dimension ref="D2:Z80"/>
+  <dimension ref="D2:AB81"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M74" sqref="M74:N75"/>
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,15 +895,16 @@
     <col min="24" max="24" width="15.7109375" customWidth="1"/>
     <col min="25" max="25" width="19.5703125" customWidth="1"/>
     <col min="26" max="26" width="35.28515625" customWidth="1"/>
+    <col min="28" max="28" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:28" x14ac:dyDescent="0.25">
       <c r="J2">
         <f>60/2.5</f>
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:28" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
         <v>65</v>
       </c>
@@ -902,7 +919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:28" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>68</v>
       </c>
@@ -913,7 +930,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:28" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
         <v>26</v>
       </c>
@@ -924,20 +941,20 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12" t="s">
+      <c r="L6" s="13"/>
+      <c r="M6" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="N6" s="12"/>
+      <c r="N6" s="13"/>
       <c r="O6" t="s">
         <v>90</v>
       </c>
@@ -948,7 +965,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
@@ -974,7 +991,7 @@
       </c>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>79</v>
       </c>
@@ -1009,7 +1026,7 @@
       </c>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>79</v>
       </c>
@@ -1020,7 +1037,7 @@
         <v>8</v>
       </c>
       <c r="H9">
-        <v>15.5</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
         <v>60</v>
@@ -1033,15 +1050,18 @@
       </c>
       <c r="M9" s="2">
         <f>($H9/$H$3)*K9</f>
-        <v>24.8</v>
+        <v>30.4</v>
       </c>
       <c r="N9" s="2">
         <f>($H9/$H$3)*L9</f>
-        <v>37.200000000000003</v>
+        <v>45.599999999999994</v>
       </c>
       <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="AB9" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>80</v>
       </c>
@@ -1097,7 +1117,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="4:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>80</v>
       </c>
@@ -1134,20 +1154,24 @@
       <c r="V11" t="s">
         <v>120</v>
       </c>
-      <c r="W11">
-        <v>3000</v>
-      </c>
-      <c r="X11">
-        <v>1500</v>
-      </c>
-      <c r="Y11">
-        <v>1500</v>
-      </c>
-      <c r="Z11">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="12" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="W11" s="2">
+        <f>SUM(N8:N16)</f>
+        <v>2927.6</v>
+      </c>
+      <c r="X11" s="2">
+        <f>N8+N9+N16</f>
+        <v>1477.6</v>
+      </c>
+      <c r="Y11" s="2">
+        <f>X11</f>
+        <v>1477.6</v>
+      </c>
+      <c r="Z11" s="2">
+        <f>Y11</f>
+        <v>1477.6</v>
+      </c>
+    </row>
+    <row r="12" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>80</v>
       </c>
@@ -1182,22 +1206,23 @@
         <v>121</v>
       </c>
       <c r="W12" s="2">
-        <f>SUM(N17:N29)</f>
-        <v>13676.8</v>
-      </c>
-      <c r="X12">
-        <v>2600</v>
+        <f>SUM(N17:N31)</f>
+        <v>12787.6</v>
+      </c>
+      <c r="X12" s="2">
+        <f>N17+N18+N19</f>
+        <v>2607.6000000000004</v>
       </c>
       <c r="Y12" s="2">
-        <f>SUM(N17:N29)</f>
-        <v>13676.8</v>
+        <f>W12</f>
+        <v>12787.6</v>
       </c>
       <c r="Z12" s="2">
-        <f>SUM(N17:N29)</f>
-        <v>13676.8</v>
-      </c>
-    </row>
-    <row r="13" spans="4:26" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Z12:Z15" si="1">Y12</f>
+        <v>12787.6</v>
+      </c>
+    </row>
+    <row r="13" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>0</v>
       </c>
@@ -1211,37 +1236,41 @@
         <v>64</v>
       </c>
       <c r="K13">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <f>H13*K13</f>
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="N13">
         <f>H13*L13</f>
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="V13" t="s">
         <v>122</v>
       </c>
-      <c r="W13">
-        <v>9500</v>
-      </c>
-      <c r="X13">
-        <v>1100</v>
+      <c r="W13" s="2">
+        <f>SUM(N32:N41)</f>
+        <v>9578.7999999999993</v>
+      </c>
+      <c r="X13" s="2">
+        <f>N32+N33</f>
+        <v>1178.8</v>
       </c>
       <c r="Y13">
-        <v>1100</v>
-      </c>
-      <c r="Z13">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="14" spans="4:26" x14ac:dyDescent="0.25">
+        <f>X13</f>
+        <v>1178.8</v>
+      </c>
+      <c r="Z13" s="2">
+        <f t="shared" si="1"/>
+        <v>1178.8</v>
+      </c>
+    </row>
+    <row r="14" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F14" s="4" t="s">
         <v>0</v>
       </c>
@@ -1263,20 +1292,24 @@
       <c r="V14" t="s">
         <v>123</v>
       </c>
-      <c r="W14">
-        <v>4000</v>
-      </c>
-      <c r="X14">
-        <v>2000</v>
+      <c r="W14" s="2">
+        <f>SUM(N42:N50)</f>
+        <v>8885</v>
+      </c>
+      <c r="X14" s="2">
+        <f>N42+N43</f>
+        <v>2020</v>
       </c>
       <c r="Y14">
-        <v>2000</v>
-      </c>
-      <c r="Z14">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="15" spans="4:26" x14ac:dyDescent="0.25">
+        <f>X14</f>
+        <v>2020</v>
+      </c>
+      <c r="Z14" s="2">
+        <f t="shared" si="1"/>
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="15" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>79</v>
       </c>
@@ -1293,18 +1326,18 @@
         <v>64</v>
       </c>
       <c r="K15">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="M15" s="2">
         <f>H15*K15</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="N15" s="2">
         <f>H15*L15</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="O15" t="s">
         <v>92</v>
@@ -1313,26 +1346,30 @@
         <v>260</v>
       </c>
       <c r="Q15" s="2">
-        <f t="shared" ref="Q15:Q63" si="1">P15-N15</f>
-        <v>-340</v>
+        <f t="shared" ref="Q15:Q64" si="2">P15-N15</f>
+        <v>260</v>
       </c>
       <c r="V15" t="s">
         <v>124</v>
       </c>
-      <c r="W15">
-        <v>22000</v>
-      </c>
-      <c r="X15">
-        <v>600</v>
+      <c r="W15" s="2">
+        <f>SUM(N55:N66)</f>
+        <v>24775.200000000001</v>
+      </c>
+      <c r="X15" s="2">
+        <f>N55+N56</f>
+        <v>625.19999999999993</v>
       </c>
       <c r="Y15">
-        <v>600</v>
-      </c>
-      <c r="Z15">
-        <v>22000</v>
-      </c>
-    </row>
-    <row r="16" spans="4:26" x14ac:dyDescent="0.25">
+        <f>X15</f>
+        <v>625.19999999999993</v>
+      </c>
+      <c r="Z15" s="2">
+        <f>W15</f>
+        <v>24775.200000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="4:28" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>0</v>
       </c>
@@ -1362,19 +1399,19 @@
       <c r="Q16" s="2"/>
       <c r="W16" s="2">
         <f>SUM(W11:W15)</f>
-        <v>52176.800000000003</v>
+        <v>58954.2</v>
       </c>
       <c r="X16" s="2">
         <f>SUM(X11:X15)</f>
-        <v>7800</v>
+        <v>7909.2</v>
       </c>
       <c r="Y16" s="2">
         <f>SUM(Y11:Y15)</f>
-        <v>18876.8</v>
+        <v>18089.2</v>
       </c>
       <c r="Z16" s="2">
         <f>SUM(Z11:Z15)</f>
-        <v>40276.800000000003</v>
+        <v>42239.199999999997</v>
       </c>
     </row>
     <row r="17" spans="4:17" x14ac:dyDescent="0.25">
@@ -1448,45 +1485,33 @@
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>79</v>
-      </c>
       <c r="F19" t="s">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="H19">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="I19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K19">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="L19">
-        <v>170</v>
+        <v>24</v>
       </c>
       <c r="M19" s="2">
-        <f>H19*K19</f>
-        <v>400</v>
+        <f>($H19/$H$3)*K19</f>
+        <v>7.2</v>
       </c>
       <c r="N19" s="2">
-        <f>H19*L19</f>
-        <v>680</v>
-      </c>
-      <c r="O19" t="s">
-        <v>92</v>
-      </c>
-      <c r="P19">
-        <v>260</v>
-      </c>
-      <c r="Q19" s="2">
-        <f t="shared" ref="Q19" si="2">P19-N19</f>
-        <v>-420</v>
-      </c>
+        <f>($H19/$H$3)*L19</f>
+        <v>10.8</v>
+      </c>
+      <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
@@ -1496,32 +1521,38 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I20" t="s">
         <v>64</v>
       </c>
-      <c r="J20" t="s">
-        <v>77</v>
-      </c>
       <c r="K20">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="L20">
-        <v>1500</v>
+        <v>170</v>
       </c>
       <c r="M20" s="2">
         <f>H20*K20</f>
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="N20" s="2">
-        <f t="shared" ref="N20:N26" si="3">$H20*L20</f>
-        <v>1500</v>
-      </c>
-      <c r="Q20" s="2"/>
+        <f>H20*L20</f>
+        <v>680</v>
+      </c>
+      <c r="O20" t="s">
+        <v>92</v>
+      </c>
+      <c r="P20">
+        <v>260</v>
+      </c>
+      <c r="Q20" s="2">
+        <f t="shared" ref="Q20" si="3">P20-N20</f>
+        <v>-420</v>
+      </c>
     </row>
     <row r="21" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
@@ -1531,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -1540,21 +1571,21 @@
         <v>64</v>
       </c>
       <c r="J21" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K21">
         <v>1000</v>
       </c>
       <c r="L21">
+        <v>1500</v>
+      </c>
+      <c r="M21" s="2">
+        <f>H21*K21</f>
         <v>1000</v>
       </c>
-      <c r="M21" s="2">
-        <f t="shared" ref="M21:M26" si="4">$H21*K21</f>
-        <v>1000</v>
-      </c>
       <c r="N21" s="2">
-        <f t="shared" si="3"/>
-        <v>1000</v>
+        <f t="shared" ref="N21:N27" si="4">$H21*L21</f>
+        <v>1500</v>
       </c>
       <c r="Q21" s="2"/>
     </row>
@@ -1566,27 +1597,30 @@
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22" t="s">
         <v>64</v>
+      </c>
+      <c r="J22" t="s">
+        <v>76</v>
       </c>
       <c r="K22">
         <v>1000</v>
       </c>
       <c r="L22">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="M22" s="2">
+        <f t="shared" ref="M22:M27" si="5">$H22*K22</f>
+        <v>1000</v>
+      </c>
+      <c r="N22" s="2">
         <f t="shared" si="4"/>
         <v>1000</v>
-      </c>
-      <c r="N22" s="2">
-        <f t="shared" si="3"/>
-        <v>1600</v>
       </c>
       <c r="Q22" s="2"/>
     </row>
@@ -1598,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -1607,18 +1641,18 @@
         <v>64</v>
       </c>
       <c r="K23">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="L23">
-        <v>100</v>
+        <v>1600</v>
       </c>
       <c r="M23" s="2">
+        <f t="shared" si="5"/>
+        <v>1000</v>
+      </c>
+      <c r="N23" s="2">
         <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="N23" s="2">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <v>1600</v>
       </c>
       <c r="Q23" s="2"/>
     </row>
@@ -1630,7 +1664,7 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -1645,11 +1679,11 @@
         <v>100</v>
       </c>
       <c r="M24" s="2">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="N24" s="2">
         <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="N24" s="2">
-        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="Q24" s="2"/>
@@ -1662,7 +1696,7 @@
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -1677,19 +1711,16 @@
         <v>100</v>
       </c>
       <c r="M25" s="2">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="N25" s="2">
         <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="N25" s="2">
-        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="Q25" s="2"/>
     </row>
     <row r="26" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>80</v>
-      </c>
       <c r="E26" t="s">
         <v>79</v>
       </c>
@@ -1697,7 +1728,7 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -1706,22 +1737,25 @@
         <v>64</v>
       </c>
       <c r="K26">
-        <v>1300</v>
+        <v>50</v>
       </c>
       <c r="L26">
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="M26" s="2">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="N26" s="2">
         <f t="shared" si="4"/>
-        <v>1300</v>
-      </c>
-      <c r="N26" s="2">
-        <f t="shared" si="3"/>
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="Q26" s="2"/>
     </row>
     <row r="27" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
       <c r="E27" t="s">
         <v>79</v>
       </c>
@@ -1729,7 +1763,7 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -1738,25 +1772,22 @@
         <v>64</v>
       </c>
       <c r="K27">
-        <v>700</v>
+        <v>1300</v>
       </c>
       <c r="L27">
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" ref="M27:M29" si="5">$H27*K27</f>
-        <v>700</v>
+        <f t="shared" si="5"/>
+        <v>1300</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" ref="N27:N29" si="6">$H27*L27</f>
-        <v>900</v>
+        <f t="shared" si="4"/>
+        <v>1500</v>
       </c>
       <c r="Q27" s="2"/>
     </row>
     <row r="28" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D28" t="s">
-        <v>80</v>
-      </c>
       <c r="E28" t="s">
         <v>79</v>
       </c>
@@ -1764,121 +1795,121 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>64</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" ref="M28:M30" si="6">$H28*K28</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" ref="N28:N30" si="7">$H28*L28</f>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="2"/>
+    </row>
+    <row r="29" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
         <v>24</v>
       </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-      <c r="I28" t="s">
-        <v>64</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29" t="s">
         <v>78</v>
       </c>
-      <c r="K28">
+      <c r="K29">
         <v>60</v>
       </c>
-      <c r="L28">
+      <c r="L29">
         <v>100</v>
       </c>
-      <c r="M28" s="2">
-        <f t="shared" si="5"/>
+      <c r="M29" s="2">
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="N28" s="2">
+      <c r="N29" s="2">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="Q29" s="2"/>
+    </row>
+    <row r="30" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>64</v>
+      </c>
+      <c r="J30" t="s">
+        <v>82</v>
+      </c>
+      <c r="K30">
+        <v>2500</v>
+      </c>
+      <c r="L30">
+        <v>3500</v>
+      </c>
+      <c r="M30" s="2">
         <f t="shared" si="6"/>
-        <v>100</v>
-      </c>
-      <c r="Q28" s="2"/>
-    </row>
-    <row r="29" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="E29" t="s">
-        <v>81</v>
-      </c>
-      <c r="F29" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" t="s">
-        <v>25</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29" t="s">
-        <v>64</v>
-      </c>
-      <c r="J29" t="s">
-        <v>82</v>
-      </c>
-      <c r="K29">
         <v>2500</v>
       </c>
-      <c r="L29">
+      <c r="N30" s="2">
+        <f t="shared" si="7"/>
         <v>3500</v>
       </c>
-      <c r="M29" s="2">
-        <f t="shared" si="5"/>
-        <v>2500</v>
-      </c>
-      <c r="N29" s="2">
-        <f t="shared" si="6"/>
-        <v>3500</v>
-      </c>
-      <c r="Q29" s="2"/>
-    </row>
-    <row r="30" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="F30" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G30" s="4" t="s">
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="4">
-        <v>1</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="Q30" s="2"/>
-    </row>
-    <row r="31" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="E31" t="s">
-        <v>79</v>
-      </c>
-      <c r="F31" t="s">
-        <v>2</v>
-      </c>
-      <c r="G31" t="s">
-        <v>26</v>
-      </c>
-      <c r="H31">
-        <v>10.9</v>
-      </c>
-      <c r="I31" t="s">
-        <v>60</v>
-      </c>
-      <c r="J31" t="s">
-        <v>72</v>
-      </c>
-      <c r="K31">
-        <v>100</v>
-      </c>
-      <c r="L31">
-        <v>100</v>
-      </c>
-      <c r="M31" s="2">
-        <f>($H31/$H$5)*K31</f>
-        <v>1090</v>
-      </c>
-      <c r="N31" s="2">
-        <f>($H31/$H$5)*L31</f>
-        <v>1090</v>
-      </c>
+      <c r="H31" s="4">
+        <v>1</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
       <c r="Q31" s="2"/>
     </row>
     <row r="32" spans="4:17" x14ac:dyDescent="0.25">
@@ -1889,78 +1920,71 @@
         <v>2</v>
       </c>
       <c r="G32" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="H32">
-        <v>32.1</v>
+        <v>10.9</v>
       </c>
       <c r="I32" t="s">
         <v>60</v>
       </c>
+      <c r="J32" t="s">
+        <v>72</v>
+      </c>
       <c r="K32">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="L32">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" ref="M32:M55" si="7">($H32/$H$3)*K32</f>
-        <v>51.36</v>
+        <f>($H32/$H$5)*K32</f>
+        <v>1090</v>
       </c>
       <c r="N32" s="2">
-        <f t="shared" ref="N32:N55" si="8">($H32/$H$3)*L32</f>
-        <v>77.039999999999992</v>
+        <f>($H32/$H$5)*L32</f>
+        <v>1090</v>
       </c>
       <c r="Q32" s="2"/>
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>79</v>
+      </c>
       <c r="F33" t="s">
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="I33" t="s">
-        <v>64</v>
-      </c>
-      <c r="J33" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="K33">
-        <v>2000</v>
+        <v>16</v>
       </c>
       <c r="L33">
-        <v>3000</v>
-      </c>
-      <c r="M33">
-        <f>$H33*K33</f>
-        <v>2000</v>
-      </c>
-      <c r="N33">
-        <f t="shared" ref="N33:N39" si="9">$H33*L33</f>
-        <v>3000</v>
-      </c>
-      <c r="O33" t="s">
-        <v>99</v>
-      </c>
-      <c r="P33">
-        <v>1000</v>
-      </c>
-      <c r="Q33" s="2">
-        <f t="shared" ref="Q33" si="10">P33-N33</f>
-        <v>-2000</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="M33" s="2">
+        <f t="shared" ref="M33:M56" si="8">($H33/$H$3)*K33</f>
+        <v>59.2</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" ref="N33:N56" si="9">($H33/$H$3)*L33</f>
+        <v>88.800000000000011</v>
+      </c>
+      <c r="Q33" s="2"/>
     </row>
     <row r="34" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="E34" s="9"/>
       <c r="F34" t="s">
         <v>2</v>
       </c>
       <c r="G34" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="H34">
         <v>1</v>
@@ -1968,48 +1992,61 @@
       <c r="I34" t="s">
         <v>64</v>
       </c>
+      <c r="J34" t="s">
+        <v>75</v>
+      </c>
       <c r="K34">
+        <v>2000</v>
+      </c>
+      <c r="L34">
         <v>3000</v>
-      </c>
-      <c r="L34">
-        <v>4500</v>
       </c>
       <c r="M34">
         <f>$H34*K34</f>
+        <v>2000</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ref="N34:N40" si="10">$H34*L34</f>
         <v>3000</v>
       </c>
-      <c r="N34">
-        <f t="shared" si="9"/>
-        <v>4500</v>
-      </c>
-      <c r="Q34" s="2"/>
+      <c r="O34" t="s">
+        <v>99</v>
+      </c>
+      <c r="P34">
+        <v>1000</v>
+      </c>
+      <c r="Q34" s="2">
+        <f t="shared" ref="Q34" si="11">P34-N34</f>
+        <v>-2000</v>
+      </c>
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E35" s="9"/>
       <c r="F35" t="s">
         <v>2</v>
       </c>
       <c r="G35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H35">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I35" t="s">
         <v>64</v>
       </c>
       <c r="K35">
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="L35">
-        <v>100</v>
+        <v>4500</v>
       </c>
       <c r="M35">
         <f>$H35*K35</f>
-        <v>900</v>
+        <v>3000</v>
       </c>
       <c r="N35">
-        <f t="shared" si="9"/>
-        <v>900</v>
+        <f t="shared" si="10"/>
+        <v>4500</v>
       </c>
       <c r="Q35" s="2"/>
     </row>
@@ -2018,27 +2055,27 @@
         <v>2</v>
       </c>
       <c r="G36" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="H36">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I36" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="K36">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L36">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M36">
-        <f t="shared" ref="M36:M39" si="11">$H36*K36</f>
-        <v>200</v>
+        <f>$H36*K36</f>
+        <v>0</v>
       </c>
       <c r="N36">
-        <f t="shared" si="9"/>
-        <v>200</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="Q36" s="2"/>
     </row>
@@ -2047,42 +2084,36 @@
         <v>2</v>
       </c>
       <c r="G37" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="K37">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="L37">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="M37">
-        <f t="shared" si="11"/>
-        <v>65</v>
+        <f t="shared" ref="M37:M40" si="12">$H37*K37</f>
+        <v>0</v>
       </c>
       <c r="N37">
-        <f t="shared" si="9"/>
-        <v>65</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="Q37" s="2"/>
     </row>
     <row r="38" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>80</v>
-      </c>
-      <c r="E38" t="s">
-        <v>79</v>
-      </c>
       <c r="F38" t="s">
         <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="H38">
         <v>1</v>
@@ -2090,108 +2121,108 @@
       <c r="I38" t="s">
         <v>64</v>
       </c>
-      <c r="J38" t="s">
-        <v>31</v>
-      </c>
       <c r="K38">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="L38">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="M38">
-        <f t="shared" si="11"/>
-        <v>150</v>
+        <f t="shared" si="12"/>
+        <v>0</v>
       </c>
       <c r="N38">
-        <f t="shared" si="9"/>
-        <v>600</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="Q38" s="2"/>
     </row>
     <row r="39" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="E39" s="10"/>
+      <c r="D39" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" t="s">
+        <v>79</v>
+      </c>
       <c r="F39" t="s">
         <v>2</v>
       </c>
       <c r="G39" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
       <c r="I39" t="s">
         <v>64</v>
+      </c>
+      <c r="J39" t="s">
+        <v>31</v>
       </c>
       <c r="K39">
         <v>150</v>
       </c>
       <c r="L39">
+        <v>600</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="12"/>
+        <v>150</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="10"/>
+        <v>600</v>
+      </c>
+      <c r="Q39" s="2"/>
+    </row>
+    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E40" s="10"/>
+      <c r="F40" t="s">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40" t="s">
+        <v>64</v>
+      </c>
+      <c r="K40">
+        <v>150</v>
+      </c>
+      <c r="L40">
         <v>300</v>
       </c>
-      <c r="M39">
-        <f t="shared" si="11"/>
+      <c r="M40">
+        <f t="shared" si="12"/>
         <v>150</v>
       </c>
-      <c r="N39">
-        <f t="shared" si="9"/>
+      <c r="N40">
+        <f t="shared" si="10"/>
         <v>300</v>
       </c>
-      <c r="Q39" s="2"/>
-    </row>
-    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="F40" s="4" t="s">
+      <c r="Q40" s="2"/>
+    </row>
+    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F41" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G41" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H40" s="4">
-        <v>1</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J40" s="4"/>
-      <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="Q40" s="2"/>
-    </row>
-    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="E41" t="s">
-        <v>79</v>
-      </c>
-      <c r="F41" t="s">
-        <v>4</v>
-      </c>
-      <c r="G41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H41">
-        <v>19</v>
-      </c>
-      <c r="I41" t="s">
-        <v>60</v>
-      </c>
-      <c r="J41" t="s">
-        <v>72</v>
-      </c>
-      <c r="K41">
-        <v>100</v>
-      </c>
-      <c r="L41">
-        <v>100</v>
-      </c>
-      <c r="M41" s="2">
-        <f>($H41/$H$5)*K41</f>
-        <v>1900</v>
-      </c>
-      <c r="N41" s="2">
-        <f>($H41/$H$5)*L41</f>
-        <v>1900</v>
-      </c>
+      <c r="H41" s="4">
+        <v>1</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
       <c r="Q41" s="2"/>
     </row>
     <row r="42" spans="4:17" x14ac:dyDescent="0.25">
@@ -2202,30 +2233,30 @@
         <v>4</v>
       </c>
       <c r="G42" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="H42">
-        <v>30.6</v>
+        <v>19</v>
       </c>
       <c r="I42" t="s">
         <v>60</v>
       </c>
       <c r="J42" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="K42">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="L42">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="M42" s="2">
-        <f t="shared" si="7"/>
-        <v>48.96</v>
+        <f>($H42/$H$5)*K42</f>
+        <v>1900</v>
       </c>
       <c r="N42" s="2">
-        <f t="shared" si="8"/>
-        <v>73.44</v>
+        <f>($H42/$H$5)*L42</f>
+        <v>1900</v>
       </c>
       <c r="Q42" s="2"/>
     </row>
@@ -2237,27 +2268,30 @@
         <v>4</v>
       </c>
       <c r="G43" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="H43">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="I43" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="J43" t="s">
+        <v>37</v>
       </c>
       <c r="K43">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="L43">
-        <v>100</v>
-      </c>
-      <c r="M43">
-        <f t="shared" ref="M43" si="12">$H43*K43</f>
-        <v>3000</v>
-      </c>
-      <c r="N43">
-        <f t="shared" ref="N43" si="13">$H43*L43</f>
-        <v>3000</v>
+        <v>24</v>
+      </c>
+      <c r="M43" s="2">
+        <f t="shared" si="8"/>
+        <v>80</v>
+      </c>
+      <c r="N43" s="2">
+        <f t="shared" si="9"/>
+        <v>120</v>
       </c>
       <c r="Q43" s="2"/>
     </row>
@@ -2269,39 +2303,39 @@
         <v>4</v>
       </c>
       <c r="G44" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="I44" t="s">
         <v>64</v>
       </c>
       <c r="K44">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="L44">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="M44">
-        <f t="shared" ref="M44:M48" si="14">$H44*K44</f>
-        <v>65</v>
+        <f t="shared" ref="M44" si="13">$H44*K44</f>
+        <v>0</v>
       </c>
       <c r="N44">
-        <f t="shared" ref="N44:N48" si="15">$H44*L44</f>
-        <v>65</v>
+        <f t="shared" ref="N44" si="14">$H44*L44</f>
+        <v>0</v>
       </c>
       <c r="Q44" s="2"/>
     </row>
     <row r="45" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F45" t="s">
         <v>4</v>
       </c>
       <c r="G45" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -2310,18 +2344,18 @@
         <v>64</v>
       </c>
       <c r="K45">
-        <v>500</v>
+        <v>65</v>
       </c>
       <c r="L45">
-        <v>1200</v>
+        <v>65</v>
       </c>
       <c r="M45">
-        <f t="shared" si="14"/>
-        <v>500</v>
+        <f t="shared" ref="M45:M49" si="15">$H45*K45</f>
+        <v>65</v>
       </c>
       <c r="N45">
-        <f t="shared" si="15"/>
-        <v>1200</v>
+        <f t="shared" ref="N45:N49" si="16">$H45*L45</f>
+        <v>65</v>
       </c>
       <c r="Q45" s="2"/>
     </row>
@@ -2333,7 +2367,7 @@
         <v>4</v>
       </c>
       <c r="G46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H46">
         <v>1</v>
@@ -2342,18 +2376,18 @@
         <v>64</v>
       </c>
       <c r="K46">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L46">
-        <v>4000</v>
+        <v>1200</v>
       </c>
       <c r="M46">
-        <f t="shared" si="14"/>
-        <v>1000</v>
+        <f t="shared" si="15"/>
+        <v>500</v>
       </c>
       <c r="N46">
-        <f t="shared" si="15"/>
-        <v>4000</v>
+        <f t="shared" si="16"/>
+        <v>1200</v>
       </c>
       <c r="Q46" s="2"/>
     </row>
@@ -2365,7 +2399,7 @@
         <v>4</v>
       </c>
       <c r="G47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -2373,108 +2407,105 @@
       <c r="I47" t="s">
         <v>64</v>
       </c>
-      <c r="J47" t="s">
-        <v>83</v>
-      </c>
       <c r="K47">
-        <v>150</v>
+        <v>1000</v>
       </c>
       <c r="L47">
-        <v>400</v>
+        <v>4000</v>
       </c>
       <c r="M47">
-        <f t="shared" si="14"/>
-        <v>150</v>
+        <f t="shared" si="15"/>
+        <v>1000</v>
       </c>
       <c r="N47">
-        <f t="shared" si="15"/>
-        <v>400</v>
+        <f t="shared" si="16"/>
+        <v>4000</v>
       </c>
       <c r="Q47" s="2"/>
     </row>
     <row r="48" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="E48" s="10"/>
+      <c r="E48" t="s">
+        <v>80</v>
+      </c>
       <c r="F48" t="s">
         <v>4</v>
       </c>
       <c r="G48" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H48">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I48" t="s">
         <v>64</v>
+      </c>
+      <c r="J48" t="s">
+        <v>83</v>
       </c>
       <c r="K48">
         <v>150</v>
       </c>
       <c r="L48">
+        <v>400</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="15"/>
+        <v>150</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="16"/>
+        <v>400</v>
+      </c>
+      <c r="Q48" s="2"/>
+    </row>
+    <row r="49" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E49" s="10"/>
+      <c r="F49" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" t="s">
+        <v>38</v>
+      </c>
+      <c r="H49">
+        <v>4</v>
+      </c>
+      <c r="I49" t="s">
+        <v>64</v>
+      </c>
+      <c r="K49">
+        <v>150</v>
+      </c>
+      <c r="L49">
         <v>300</v>
       </c>
-      <c r="M48">
-        <f t="shared" si="14"/>
+      <c r="M49">
+        <f t="shared" si="15"/>
         <v>600</v>
       </c>
-      <c r="N48">
-        <f t="shared" si="15"/>
+      <c r="N49">
+        <f t="shared" si="16"/>
         <v>1200</v>
       </c>
-      <c r="Q48" s="2"/>
-    </row>
-    <row r="49" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="F49" s="4" t="s">
+      <c r="Q49" s="2"/>
+    </row>
+    <row r="50" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="F50" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="G50" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H49" s="4">
-        <v>1</v>
-      </c>
-      <c r="I49" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="Q49" s="2"/>
-    </row>
-    <row r="50" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="E50" t="s">
-        <v>79</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="2">
-        <v>18.5</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K50" s="2">
-        <v>100</v>
-      </c>
-      <c r="L50" s="2">
-        <v>108</v>
-      </c>
-      <c r="M50" s="2">
-        <f>($H50/$H$4)*K50</f>
-        <v>1850</v>
-      </c>
-      <c r="N50" s="2">
-        <f>($H50/$H$4)*L50</f>
-        <v>1998</v>
-      </c>
+      <c r="H50" s="4">
+        <v>1</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
       <c r="Q50" s="2"/>
     </row>
     <row r="51" spans="4:17" x14ac:dyDescent="0.25">
@@ -2485,30 +2516,30 @@
         <v>5</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H51" s="2">
-        <v>56</v>
+        <v>18.5</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>60</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K51" s="2">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="L51" s="2">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="M51" s="2">
-        <f t="shared" si="7"/>
-        <v>89.6</v>
+        <f>($H51/$H$4)*K51</f>
+        <v>1850</v>
       </c>
       <c r="N51" s="2">
-        <f t="shared" si="8"/>
-        <v>134.39999999999998</v>
+        <f>($H51/$H$4)*L51</f>
+        <v>1998</v>
       </c>
       <c r="Q51" s="2"/>
     </row>
@@ -2520,30 +2551,30 @@
         <v>5</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="H52" s="2">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K52" s="2">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="L52" s="2">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="M52" s="2">
-        <f>$H52*K52</f>
-        <v>100</v>
+        <f t="shared" si="8"/>
+        <v>89.6</v>
       </c>
       <c r="N52" s="2">
-        <f>$H52*L52</f>
-        <v>100</v>
+        <f t="shared" si="9"/>
+        <v>134.39999999999998</v>
       </c>
       <c r="Q52" s="2"/>
     </row>
@@ -2552,10 +2583,10 @@
         <v>79</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="H53" s="2">
         <v>1</v>
@@ -2564,21 +2595,21 @@
         <v>64</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K53" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L53" s="2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M53" s="2">
         <f>$H53*K53</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="N53" s="2">
-        <f t="shared" ref="N53" si="16">$H53*L53</f>
-        <v>100</v>
+        <f>$H53*L53</f>
+        <v>0</v>
       </c>
       <c r="Q53" s="2"/>
     </row>
@@ -2587,33 +2618,33 @@
         <v>79</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="H54" s="2">
-        <v>5.3</v>
+        <v>1</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="K54" s="2">
         <v>100</v>
       </c>
       <c r="L54" s="2">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="M54" s="2">
-        <f>($H54/$H$4)*K54</f>
-        <v>530</v>
+        <f>$H54*K54</f>
+        <v>100</v>
       </c>
       <c r="N54" s="2">
-        <f>($H54/$H$4)*L54</f>
-        <v>572.4</v>
+        <f t="shared" ref="N54" si="17">$H54*L54</f>
+        <v>100</v>
       </c>
       <c r="Q54" s="2"/>
     </row>
@@ -2621,115 +2652,106 @@
       <c r="E55" t="s">
         <v>79</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K55" s="2">
+        <v>100</v>
+      </c>
+      <c r="L55" s="2">
+        <v>108</v>
+      </c>
+      <c r="M55" s="2">
+        <f>($H55/$H$4)*K55</f>
+        <v>530</v>
+      </c>
+      <c r="N55" s="2">
+        <f>($H55/$H$4)*L55</f>
+        <v>572.4</v>
+      </c>
+      <c r="Q55" s="2"/>
+    </row>
+    <row r="56" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>79</v>
+      </c>
+      <c r="F56" t="s">
+        <v>3</v>
+      </c>
+      <c r="G56" t="s">
         <v>8</v>
       </c>
-      <c r="H55">
-        <v>16.7</v>
-      </c>
-      <c r="I55" t="s">
+      <c r="H56">
+        <v>22</v>
+      </c>
+      <c r="I56" t="s">
         <v>60</v>
       </c>
-      <c r="K55">
+      <c r="K56">
         <v>16</v>
       </c>
-      <c r="L55">
+      <c r="L56">
         <v>24</v>
       </c>
-      <c r="M55" s="2">
-        <f t="shared" si="7"/>
-        <v>26.72</v>
-      </c>
-      <c r="N55" s="2">
+      <c r="M56" s="2">
         <f t="shared" si="8"/>
-        <v>40.08</v>
-      </c>
-      <c r="Q55" s="2"/>
-    </row>
-    <row r="56" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="N56" s="2">
+        <f t="shared" si="9"/>
+        <v>52.800000000000004</v>
+      </c>
+      <c r="Q56" s="2"/>
+    </row>
+    <row r="57" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
         <v>79</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E57" t="s">
         <v>80</v>
       </c>
-      <c r="F56" s="6" t="s">
+      <c r="F57" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="G57" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H56" s="6">
-        <v>1</v>
-      </c>
-      <c r="I56" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J56" s="6" t="s">
+      <c r="H57" s="6">
+        <v>1</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J57" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="K56" s="6">
+      <c r="K57" s="6">
         <v>9400</v>
       </c>
-      <c r="L56" s="6">
+      <c r="L57" s="6">
         <v>10000</v>
       </c>
-      <c r="M56" s="7">
-        <f t="shared" ref="M56" si="17">$H56*K56</f>
+      <c r="M57" s="7">
+        <f t="shared" ref="M57" si="18">$H57*K57</f>
         <v>9400</v>
       </c>
-      <c r="N56" s="7">
-        <f t="shared" ref="N56" si="18">$H56*L56</f>
+      <c r="N57" s="7">
+        <f t="shared" ref="N57" si="19">$H57*L57</f>
         <v>10000</v>
       </c>
-      <c r="Q56" s="2"/>
-    </row>
-    <row r="57" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="E57" t="s">
-        <v>81</v>
-      </c>
-      <c r="F57" t="s">
-        <v>3</v>
-      </c>
-      <c r="G57" t="s">
-        <v>44</v>
-      </c>
-      <c r="H57">
-        <v>1</v>
-      </c>
-      <c r="I57" t="s">
-        <v>64</v>
-      </c>
-      <c r="J57" t="s">
-        <v>47</v>
-      </c>
-      <c r="K57" s="6">
-        <v>2000</v>
-      </c>
-      <c r="L57" s="6">
-        <v>3500</v>
-      </c>
-      <c r="M57" s="2">
-        <f t="shared" ref="M57:M60" si="19">$H57*K57</f>
-        <v>2000</v>
-      </c>
-      <c r="N57" s="2">
-        <f t="shared" ref="N57:N60" si="20">$H57*L57</f>
-        <v>3500</v>
-      </c>
-      <c r="O57" t="s">
-        <v>93</v>
-      </c>
-      <c r="P57">
-        <v>2900</v>
-      </c>
-      <c r="Q57" s="2">
-        <f t="shared" si="1"/>
-        <v>-600</v>
-      </c>
+      <c r="Q57" s="2"/>
     </row>
     <row r="58" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
@@ -2739,7 +2761,7 @@
         <v>3</v>
       </c>
       <c r="G58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H58">
         <v>1</v>
@@ -2751,27 +2773,27 @@
         <v>47</v>
       </c>
       <c r="K58" s="6">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="L58" s="6">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="M58" s="2">
-        <f t="shared" si="19"/>
-        <v>1500</v>
+        <f t="shared" ref="M58:M61" si="20">$H58*K58</f>
+        <v>2000</v>
       </c>
       <c r="N58" s="2">
-        <f t="shared" si="20"/>
-        <v>2500</v>
+        <f t="shared" ref="N58:N61" si="21">$H58*L58</f>
+        <v>3500</v>
       </c>
       <c r="O58" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P58">
-        <v>1900</v>
+        <v>2900</v>
       </c>
       <c r="Q58" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-600</v>
       </c>
     </row>
@@ -2783,7 +2805,7 @@
         <v>3</v>
       </c>
       <c r="G59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -2795,20 +2817,29 @@
         <v>47</v>
       </c>
       <c r="K59" s="6">
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="L59" s="6">
-        <v>1700</v>
+        <v>2500</v>
       </c>
       <c r="M59" s="2">
-        <f t="shared" si="19"/>
-        <v>900</v>
+        <f t="shared" si="20"/>
+        <v>1500</v>
       </c>
       <c r="N59" s="2">
-        <f t="shared" si="20"/>
-        <v>1700</v>
-      </c>
-      <c r="Q59" s="2"/>
+        <f t="shared" si="21"/>
+        <v>2500</v>
+      </c>
+      <c r="O59" t="s">
+        <v>96</v>
+      </c>
+      <c r="P59">
+        <v>1900</v>
+      </c>
+      <c r="Q59" s="2">
+        <f t="shared" si="2"/>
+        <v>-600</v>
+      </c>
     </row>
     <row r="60" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
@@ -2818,7 +2849,7 @@
         <v>3</v>
       </c>
       <c r="G60" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -2830,29 +2861,20 @@
         <v>47</v>
       </c>
       <c r="K60" s="6">
-        <v>1500</v>
+        <v>900</v>
       </c>
       <c r="L60" s="6">
-        <v>2300</v>
+        <v>1700</v>
       </c>
       <c r="M60" s="2">
-        <f t="shared" si="19"/>
-        <v>1500</v>
+        <f t="shared" si="20"/>
+        <v>900</v>
       </c>
       <c r="N60" s="2">
-        <f t="shared" si="20"/>
-        <v>2300</v>
-      </c>
-      <c r="O60" t="s">
-        <v>94</v>
-      </c>
-      <c r="P60">
-        <v>1300</v>
-      </c>
-      <c r="Q60" s="2">
-        <f t="shared" si="1"/>
-        <v>-1000</v>
-      </c>
+        <f t="shared" si="21"/>
+        <v>1700</v>
+      </c>
+      <c r="Q60" s="2"/>
     </row>
     <row r="61" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
@@ -2862,7 +2884,7 @@
         <v>3</v>
       </c>
       <c r="G61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -2871,31 +2893,31 @@
         <v>64</v>
       </c>
       <c r="J61" t="s">
-        <v>50</v>
-      </c>
-      <c r="K61">
-        <v>500</v>
-      </c>
-      <c r="L61">
-        <v>1600</v>
+        <v>47</v>
+      </c>
+      <c r="K61" s="6">
+        <v>1500</v>
+      </c>
+      <c r="L61" s="6">
+        <v>2300</v>
       </c>
       <c r="M61" s="2">
-        <f t="shared" ref="M61:N65" si="21">$H61*K61</f>
-        <v>500</v>
+        <f t="shared" si="20"/>
+        <v>1500</v>
       </c>
       <c r="N61" s="2">
         <f t="shared" si="21"/>
-        <v>1600</v>
+        <v>2300</v>
       </c>
       <c r="O61" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="P61">
-        <v>1400</v>
+        <v>1300</v>
       </c>
       <c r="Q61" s="2">
-        <f t="shared" si="1"/>
-        <v>-200</v>
+        <f t="shared" si="2"/>
+        <v>-1000</v>
       </c>
     </row>
     <row r="62" spans="4:17" x14ac:dyDescent="0.25">
@@ -2906,7 +2928,7 @@
         <v>3</v>
       </c>
       <c r="G62" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H62">
         <v>1</v>
@@ -2914,21 +2936,33 @@
       <c r="I62" t="s">
         <v>64</v>
       </c>
+      <c r="J62" t="s">
+        <v>50</v>
+      </c>
       <c r="K62">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="L62">
-        <v>150</v>
+        <v>1600</v>
       </c>
       <c r="M62" s="2">
-        <f t="shared" si="21"/>
-        <v>100</v>
+        <f t="shared" ref="M62:N66" si="22">$H62*K62</f>
+        <v>500</v>
       </c>
       <c r="N62" s="2">
-        <f t="shared" si="21"/>
-        <v>150</v>
-      </c>
-      <c r="Q62" s="2"/>
+        <f t="shared" si="22"/>
+        <v>1600</v>
+      </c>
+      <c r="O62" t="s">
+        <v>98</v>
+      </c>
+      <c r="P62">
+        <v>1400</v>
+      </c>
+      <c r="Q62" s="2">
+        <f t="shared" si="2"/>
+        <v>-200</v>
+      </c>
     </row>
     <row r="63" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
@@ -2938,7 +2972,7 @@
         <v>3</v>
       </c>
       <c r="G63" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H63">
         <v>1</v>
@@ -2947,39 +2981,30 @@
         <v>64</v>
       </c>
       <c r="K63">
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="L63">
-        <v>1900</v>
+        <v>150</v>
       </c>
       <c r="M63" s="2">
-        <f t="shared" si="21"/>
-        <v>1500</v>
+        <f t="shared" si="22"/>
+        <v>100</v>
       </c>
       <c r="N63" s="2">
-        <f t="shared" si="21"/>
-        <v>1900</v>
-      </c>
-      <c r="O63" t="s">
-        <v>97</v>
-      </c>
-      <c r="P63">
-        <v>2000</v>
-      </c>
-      <c r="Q63" s="2">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
+        <f t="shared" si="22"/>
+        <v>150</v>
+      </c>
+      <c r="Q63" s="2"/>
     </row>
     <row r="64" spans="4:17" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F64" t="s">
         <v>3</v>
       </c>
       <c r="G64" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -2988,187 +3013,228 @@
         <v>64</v>
       </c>
       <c r="K64">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="L64">
-        <v>500</v>
+        <v>1900</v>
       </c>
       <c r="M64" s="2">
-        <f t="shared" si="21"/>
-        <v>500</v>
+        <f t="shared" si="22"/>
+        <v>1500</v>
       </c>
       <c r="N64" s="2">
-        <f t="shared" si="21"/>
-        <v>500</v>
+        <f t="shared" si="22"/>
+        <v>1900</v>
       </c>
       <c r="O64" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="P64">
-        <v>260</v>
+        <v>2000</v>
       </c>
       <c r="Q64" s="2">
-        <f t="shared" ref="Q64" si="22">P64-N64</f>
-        <v>-240</v>
-      </c>
-    </row>
-    <row r="65" spans="6:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>79</v>
+      </c>
       <c r="F65" t="s">
         <v>3</v>
       </c>
       <c r="G65" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65" t="s">
+        <v>64</v>
+      </c>
+      <c r="K65">
+        <v>500</v>
+      </c>
+      <c r="L65">
+        <v>500</v>
+      </c>
+      <c r="M65" s="2">
+        <f t="shared" si="22"/>
+        <v>500</v>
+      </c>
+      <c r="N65" s="2">
+        <f t="shared" si="22"/>
+        <v>500</v>
+      </c>
+      <c r="O65" t="s">
+        <v>92</v>
+      </c>
+      <c r="P65">
+        <v>260</v>
+      </c>
+      <c r="Q65" s="2">
+        <f t="shared" ref="Q65" si="23">P65-N65</f>
+        <v>-240</v>
+      </c>
+    </row>
+    <row r="66" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>3</v>
+      </c>
+      <c r="G66" t="s">
         <v>54</v>
       </c>
-      <c r="H65">
+      <c r="H66">
         <v>3</v>
       </c>
-      <c r="I65" t="s">
-        <v>64</v>
-      </c>
-      <c r="J65" t="s">
+      <c r="I66" t="s">
+        <v>64</v>
+      </c>
+      <c r="J66" t="s">
         <v>55</v>
       </c>
-      <c r="K65">
-        <v>100</v>
-      </c>
-      <c r="L65">
-        <v>100</v>
-      </c>
-      <c r="M65">
-        <f t="shared" si="21"/>
-        <v>300</v>
-      </c>
-      <c r="N65">
-        <f t="shared" si="21"/>
-        <v>300</v>
-      </c>
-      <c r="Q65" s="2"/>
-    </row>
-    <row r="66" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F66" s="13" t="s">
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="Q66" s="2"/>
+    </row>
+    <row r="67" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F67" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="13"/>
-      <c r="K66" s="13"/>
-      <c r="L66" s="13"/>
-      <c r="M66" s="11">
-        <f>SUM(M8:M65)</f>
-        <v>48876.44</v>
-      </c>
-      <c r="N66" s="11">
-        <f>SUM(N8:N65)</f>
-        <v>67226.36</v>
-      </c>
-      <c r="P66" s="2">
-        <f>SUM(P8:P65)</f>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="11">
+        <f>SUM(M8:M66)</f>
+        <v>43106.6</v>
+      </c>
+      <c r="N67" s="11">
+        <f>SUM(N8:N66)</f>
+        <v>61186.600000000006</v>
+      </c>
+      <c r="P67" s="2">
+        <f>SUM(P8:P66)</f>
         <v>12280</v>
       </c>
-      <c r="Q66" s="2">
-        <f>SUM(Q8:Q65)</f>
-        <v>-5600</v>
-      </c>
-    </row>
-    <row r="67" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F67" s="12" t="s">
+      <c r="Q67" s="2">
+        <f>SUM(Q8:Q66)</f>
+        <v>-5000</v>
+      </c>
+    </row>
+    <row r="68" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F68" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G67" s="12"/>
-      <c r="H67" s="12"/>
-      <c r="I67" s="12"/>
-      <c r="J67" s="12"/>
-      <c r="K67" s="12"/>
-      <c r="L67" s="12"/>
-      <c r="M67" s="2">
-        <f>SUM(M8:M65)-SUM(M50:M52)</f>
-        <v>46836.840000000004</v>
-      </c>
-      <c r="N67" s="2">
-        <f>SUM(N8:N65)-SUM(N50:N52)</f>
-        <v>64993.96</v>
-      </c>
-    </row>
-    <row r="68" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F68" s="12" t="s">
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13"/>
+      <c r="L68" s="13"/>
+      <c r="M68" s="2">
+        <f>SUM(M8:M66)-SUM(M51:M53)</f>
+        <v>41167</v>
+      </c>
+      <c r="N68" s="2">
+        <f>SUM(N8:N66)-SUM(N51:N53)</f>
+        <v>59054.200000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="F69" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
-      <c r="I68" s="12"/>
-      <c r="J68" s="12"/>
-      <c r="K68" s="12"/>
-      <c r="L68" s="12"/>
-      <c r="M68" s="2">
-        <f>SUM(M50:M52)</f>
-        <v>2039.6</v>
-      </c>
-      <c r="N68" s="2">
-        <f>SUM(N50:N52)</f>
-        <v>2232.4</v>
-      </c>
-    </row>
-    <row r="74" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="M74" t="s">
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13"/>
+      <c r="L69" s="13"/>
+      <c r="M69" s="2">
+        <f>SUM(M51:M53)</f>
+        <v>1939.6</v>
+      </c>
+      <c r="N69" s="2">
+        <f>SUM(N51:N53)</f>
+        <v>2132.4</v>
+      </c>
+    </row>
+    <row r="75" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M75" t="s">
         <v>3</v>
       </c>
-      <c r="N74" s="2">
-        <f>SUM(N54:N65)</f>
-        <v>25062.48</v>
-      </c>
-    </row>
-    <row r="75" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="M75" t="s">
+      <c r="N75" s="2">
+        <f>SUM(N55:N66)</f>
+        <v>24775.200000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M76" t="s">
         <v>87</v>
       </c>
-      <c r="N75" s="2">
-        <f>SUM(N17:N30)</f>
-        <v>13676.8</v>
-      </c>
-    </row>
-    <row r="76" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="M76" t="s">
+      <c r="N76" s="2">
+        <f>SUM(N17:N31)</f>
+        <v>12787.6</v>
+      </c>
+    </row>
+    <row r="77" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M77" t="s">
         <v>88</v>
       </c>
-      <c r="N76" s="2">
-        <f>SUM(N41:N49)</f>
-        <v>11838.44</v>
-      </c>
-    </row>
-    <row r="77" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="M77" t="s">
+      <c r="N77" s="2">
+        <f>SUM(N42:N50)</f>
+        <v>8885</v>
+      </c>
+    </row>
+    <row r="78" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M78" t="s">
         <v>89</v>
       </c>
-      <c r="N77" s="2">
+      <c r="N78" s="2">
         <f>SUM(N8:N16)</f>
-        <v>3584.2</v>
-      </c>
-    </row>
-    <row r="78" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="M78" t="s">
+        <v>2927.6</v>
+      </c>
+    </row>
+    <row r="79" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M79" t="s">
         <v>2</v>
       </c>
-      <c r="N78" s="2">
-        <f>SUM(N31:N40)</f>
-        <v>10732.04</v>
-      </c>
-    </row>
-    <row r="79" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="M79" t="s">
+      <c r="N79" s="2">
+        <f>SUM(N32:N41)</f>
+        <v>9578.7999999999993</v>
+      </c>
+    </row>
+    <row r="80" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="M80" t="s">
         <v>5</v>
       </c>
-      <c r="N79" s="2">
-        <f>SUM(N50:N52)</f>
-        <v>2232.4</v>
-      </c>
-    </row>
-    <row r="80" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="M80" t="s">
+      <c r="N80" s="2">
+        <f>SUM(N51:N53)</f>
+        <v>2132.4</v>
+      </c>
+    </row>
+    <row r="81" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M81" t="s">
         <v>6</v>
       </c>
-      <c r="N80" s="2">
-        <f>SUM(N53)</f>
+      <c r="N81" s="2">
+        <f>SUM(N54)</f>
         <v>100</v>
       </c>
     </row>
@@ -3176,9 +3242,9 @@
   <mergeCells count="5">
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="M6:N6"/>
+    <mergeCell ref="F68:L68"/>
+    <mergeCell ref="F69:L69"/>
     <mergeCell ref="F67:L67"/>
-    <mergeCell ref="F68:L68"/>
-    <mergeCell ref="F66:L66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3367,7 +3433,7 @@
   <dimension ref="G7:Y20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3389,7 +3455,7 @@
       <c r="H7">
         <v>23000</v>
       </c>
-      <c r="Q7" s="14">
+      <c r="Q7" s="12">
         <v>43296</v>
       </c>
       <c r="R7">
@@ -3397,7 +3463,7 @@
       </c>
     </row>
     <row r="8" spans="7:25" x14ac:dyDescent="0.25">
-      <c r="Q8" s="14">
+      <c r="Q8" s="12">
         <v>43327</v>
       </c>
       <c r="R8">
@@ -3409,11 +3475,11 @@
       </c>
     </row>
     <row r="9" spans="7:25" x14ac:dyDescent="0.25">
-      <c r="Q9" s="14">
+      <c r="Q9" s="12">
         <v>43358</v>
       </c>
       <c r="R9">
-        <f t="shared" ref="R9:R26" si="0">R8+10000</f>
+        <f t="shared" ref="R9:R20" si="0">R8+10000</f>
         <v>120000</v>
       </c>
       <c r="S9" t="s">
@@ -3437,104 +3503,118 @@
         <v>129</v>
       </c>
       <c r="R10">
+        <v>120000</v>
+      </c>
+      <c r="S10" t="s">
+        <v>139</v>
+      </c>
+      <c r="T10" t="s">
+        <v>143</v>
+      </c>
+      <c r="X10" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="Q11" s="12">
+        <v>43419</v>
+      </c>
+      <c r="R11">
         <f t="shared" si="0"/>
         <v>130000</v>
       </c>
-      <c r="X10" t="s">
-        <v>135</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="7:25" x14ac:dyDescent="0.25">
-      <c r="Q11" s="14">
-        <v>43419</v>
-      </c>
-      <c r="R11">
+      <c r="T11" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="Q12" s="12">
+        <v>43449</v>
+      </c>
+      <c r="R12">
         <f t="shared" si="0"/>
         <v>140000</v>
       </c>
-    </row>
-    <row r="12" spans="7:25" x14ac:dyDescent="0.25">
-      <c r="Q12" s="14">
-        <v>43449</v>
-      </c>
-      <c r="R12">
+      <c r="T12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="Q13" s="12">
+        <v>43480</v>
+      </c>
+      <c r="R13">
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-    </row>
-    <row r="13" spans="7:25" x14ac:dyDescent="0.25">
-      <c r="Q13" s="14">
-        <v>43480</v>
-      </c>
-      <c r="R13">
+      <c r="T13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="Q14" s="12">
+        <v>43511</v>
+      </c>
+      <c r="R14">
         <f t="shared" si="0"/>
         <v>160000</v>
       </c>
     </row>
-    <row r="14" spans="7:25" x14ac:dyDescent="0.25">
-      <c r="Q14" s="14">
-        <v>43511</v>
-      </c>
-      <c r="R14">
+    <row r="15" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="Q15" s="12">
+        <v>43539</v>
+      </c>
+      <c r="R15">
         <f t="shared" si="0"/>
         <v>170000</v>
       </c>
     </row>
-    <row r="15" spans="7:25" x14ac:dyDescent="0.25">
-      <c r="Q15" s="14">
-        <v>43539</v>
-      </c>
-      <c r="R15">
+    <row r="16" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="Q16" s="12">
+        <v>43570</v>
+      </c>
+      <c r="R16">
         <f t="shared" si="0"/>
         <v>180000</v>
       </c>
     </row>
-    <row r="16" spans="7:25" x14ac:dyDescent="0.25">
-      <c r="Q16" s="14">
-        <v>43570</v>
-      </c>
-      <c r="R16">
+    <row r="17" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q17" s="12">
+        <v>43600</v>
+      </c>
+      <c r="R17">
         <f t="shared" si="0"/>
         <v>190000</v>
       </c>
     </row>
-    <row r="17" spans="17:18" x14ac:dyDescent="0.25">
-      <c r="Q17" s="14">
-        <v>43600</v>
-      </c>
-      <c r="R17">
+    <row r="18" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q18" s="12">
+        <v>43631</v>
+      </c>
+      <c r="R18">
         <f t="shared" si="0"/>
         <v>200000</v>
       </c>
     </row>
-    <row r="18" spans="17:18" x14ac:dyDescent="0.25">
-      <c r="Q18" s="14">
-        <v>43631</v>
-      </c>
-      <c r="R18">
+    <row r="19" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q19" s="12">
+        <v>43661</v>
+      </c>
+      <c r="R19">
         <f t="shared" si="0"/>
         <v>210000</v>
       </c>
     </row>
-    <row r="19" spans="17:18" x14ac:dyDescent="0.25">
-      <c r="Q19" s="14">
-        <v>43661</v>
-      </c>
-      <c r="R19">
+    <row r="20" spans="17:18" x14ac:dyDescent="0.25">
+      <c r="Q20" s="12">
+        <v>43692</v>
+      </c>
+      <c r="R20">
         <f t="shared" si="0"/>
         <v>220000</v>
-      </c>
-    </row>
-    <row r="20" spans="17:18" x14ac:dyDescent="0.25">
-      <c r="Q20" s="14">
-        <v>43692</v>
-      </c>
-      <c r="R20">
-        <f t="shared" si="0"/>
-        <v>230000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>